<commit_message>
meeting 01.07. todo update
</commit_message>
<xml_diff>
--- a/todo_neu.xlsx
+++ b/todo_neu.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\empschulml\Documents\GitHub\Mandy-PhD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gk42fezo\Documents\GitHub\Mandy-PhD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDBAAF2E-43D9-44EB-A8EA-02109FE0FA13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFE2E2A-5B7E-403A-8F21-7423DDBC5B5B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="5355" xr2:uid="{437BB29D-C085-46B0-AB3F-775756C491F0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16760" windowHeight="5360" xr2:uid="{437BB29D-C085-46B0-AB3F-775756C491F0}"/>
   </bookViews>
   <sheets>
     <sheet name="to dos" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>Erledigt</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Fragen an Anne notiert</t>
   </si>
   <si>
-    <t>GLMM-Artikel lesen + verstehen</t>
-  </si>
-  <si>
     <t>Infos über Journals in einem Doc zusammengestellt</t>
   </si>
   <si>
@@ -111,9 +108,6 @@
     <t>überarbeitet mit neuer Laborstudie, ET genauer beschrieben</t>
   </si>
   <si>
-    <t>ziehe aus den drei Journals wenn möglich je eine eyetracking studie, UND suche eine Bildungswissenschaftliche Studie in der Tobii Glasses benutzt wurden, lege die paper als pdf im paperordner in einen unterordner "examples" ab</t>
-  </si>
-  <si>
     <t>Fragen</t>
   </si>
   <si>
@@ -127,6 +121,27 @@
   </si>
   <si>
     <t>Forschungsliteratur zu ET einbeziehen expert-novice</t>
+  </si>
+  <si>
+    <t>Webseite: Banner und Text für "projekte"…bild mobile lab o.ä.</t>
+  </si>
+  <si>
+    <t>Webseite: einladungstext für deinen Pilot schreiben, vielleicht Bild dazu, ähnlich dem Text für Mockdataparty</t>
+  </si>
+  <si>
+    <t>UND suche eine Bildungswissenschaftliche Studie in der Tobii Glasses benutzt wurden, lege</t>
+  </si>
+  <si>
+    <t>Tobii Glasses Paper irgendwoher</t>
+  </si>
+  <si>
+    <t>Methodsection: Brille beschreiben</t>
+  </si>
+  <si>
+    <t>Eineleitung: Beispielpaper in einpflegen</t>
+  </si>
+  <si>
+    <t>LMM-Artikel lesen + verstehen</t>
   </si>
 </sst>
 </file>
@@ -549,22 +564,22 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="4" style="4" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" style="4" customWidth="1"/>
     <col min="3" max="3" width="28" style="4" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="40.85546875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="10.85546875" style="4"/>
+    <col min="4" max="4" width="27.7265625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="40.81640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="27.81640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="25.54296875" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="10.81640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -584,13 +599,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="4" t="s">
@@ -606,7 +621,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="3"/>
       <c r="C4" s="4" t="s">
@@ -623,7 +638,7 @@
       </c>
       <c r="H4" s="12"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
       <c r="C5" s="4" t="s">
@@ -637,11 +652,11 @@
       </c>
       <c r="H5" s="12"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>20</v>
@@ -650,94 +665,97 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
+      <c r="C7" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="E7" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
       <c r="E8" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:8" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="9">
         <v>1</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="4" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="9">
         <v>2</v>
       </c>
       <c r="B14" s="9"/>
       <c r="D14" s="4" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="9">
         <v>3</v>
       </c>
       <c r="B15" s="9"/>
       <c r="D15" s="4" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="9">
         <v>4</v>
       </c>
@@ -749,13 +767,13 @@
         <v>12</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="9">
         <v>5</v>
       </c>
@@ -773,86 +791,86 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="9">
         <v>6</v>
       </c>
       <c r="B18" s="9"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="9">
         <v>7</v>
       </c>
       <c r="B19" s="9"/>
     </row>
-    <row r="20" spans="1:7" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="11"/>
       <c r="B21" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="11"/>
       <c r="B22" s="11"/>
       <c r="E22" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="11"/>
       <c r="B23" s="11"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="11"/>
       <c r="B24" s="11"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="11"/>
       <c r="B25" s="11"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="11"/>
       <c r="B26" s="11"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="11"/>
       <c r="B28" s="11"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="11"/>
       <c r="B29" s="11"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="11"/>
       <c r="B30" s="11"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="11"/>
       <c r="B31" s="11"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="11"/>
       <c r="B32" s="11"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="11"/>
       <c r="B33" s="11"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="11"/>
       <c r="B34" s="11"/>
     </row>

</xml_diff>